<commit_message>
added stuff to results and performance section
</commit_message>
<xml_diff>
--- a/data/performance.xlsx
+++ b/data/performance.xlsx
@@ -751,6 +751,80 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>27.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>13 Syllables</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$20:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$N$20:$N$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1951.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>288978.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>288978.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>277609.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1781,7 +1855,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B23" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>

</xml_diff>